<commit_message>
tests; updated test data
</commit_message>
<xml_diff>
--- a/tests/tests_unit/rules/test_importers/excel_importer_data/invalid_property_dms_rules.xlsx
+++ b/tests/tests_unit/rules/test_importers/excel_importer_data/invalid_property_dms_rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\tests\tests_unit\rules\test_importers\excel_importer_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CF5132-1F56-4049-A89D-22777DF84589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5F2413-31DB-4533-98C3-1966D65B0FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>Relation</t>
-  </si>
-  <si>
-    <t>Nullable</t>
   </si>
   <si>
     <t>Default</t>
@@ -144,13 +141,16 @@
     <t>Property (linage)</t>
   </si>
   <si>
-    <t>Is List</t>
-  </si>
-  <si>
     <t>Container Property</t>
   </si>
   <si>
     <t>View Property</t>
+  </si>
+  <si>
+    <t>Min Count</t>
+  </si>
+  <si>
+    <t>Max Count</t>
   </si>
 </sst>
 </file>
@@ -601,10 +601,10 @@
     </row>
     <row r="2" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -612,7 +612,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -638,10 +638,10 @@
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -667,7 +667,7 @@
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="5"/>
@@ -694,10 +694,10 @@
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -726,7 +726,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -752,10 +752,10 @@
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -781,7 +781,7 @@
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="14">
         <v>45351.489040733439</v>
@@ -8457,7 +8457,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="20"/>
@@ -8485,16 +8485,16 @@
     </row>
     <row r="2" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -8502,10 +8502,10 @@
     </row>
     <row r="3" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="10"/>
     </row>
@@ -9522,8 +9522,8 @@
   </sheetPr>
   <dimension ref="A1:W1010"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:O2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9572,10 +9572,10 @@
     </row>
     <row r="2" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>6</v>
@@ -9587,34 +9587,34 @@
         <v>8</v>
       </c>
       <c r="F2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="I2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" s="8" t="s">
+      <c r="N2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="N2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>15</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -9627,34 +9627,34 @@
     </row>
     <row r="3" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
-        <v>17</v>
+      <c r="F3">
+        <v>0</v>
       </c>
-      <c r="F3" t="b">
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R3" s="10"/>
       <c r="S3" s="10"/>
@@ -9673,31 +9673,31 @@
     </row>
     <row r="5" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
         <v>33</v>
       </c>
-      <c r="F5" t="b">
-        <v>1</v>
+      <c r="J5" t="s">
+        <v>30</v>
       </c>
-      <c r="G5" t="s">
+      <c r="K5" t="s">
         <v>34</v>
       </c>
-      <c r="J5" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" t="s">
-        <v>35</v>
-      </c>
       <c r="L5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
@@ -22301,7 +22301,7 @@
   </sheetPr>
   <dimension ref="A1:X1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
@@ -22318,7 +22318,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -22346,16 +22346,16 @@
     </row>
     <row r="2" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -22363,10 +22363,10 @@
     </row>
     <row r="3" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" s="10"/>
     </row>

</xml_diff>